<commit_message>
update class and studentlis query
</commit_message>
<xml_diff>
--- a/Yapılacaklar.xlsx
+++ b/Yapılacaklar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7296" windowWidth="22260" windowHeight="12648" tabRatio="555"/>
+    <workbookView xWindow="0" yWindow="7752" windowWidth="22260" windowHeight="12648" tabRatio="555"/>
   </bookViews>
   <sheets>
     <sheet name="Yapilacaklar" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="141">
   <si>
     <t>Kullanıcılar</t>
   </si>
@@ -230,9 +230,6 @@
     <t>dönem yillar texfield charfield olacak ve limitlenecek burada  default olarak o yılın donemi gelebilir 2021-2022 gibi</t>
   </si>
   <si>
-    <t>burayı düzeltmek gerekiyor</t>
-  </si>
-  <si>
     <t>kullanıcılarda ilişki düzelecek birden falza kişi aynı bransı secebilecek</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>öğrencilerde ve kullanıcılarda cinsiyet olacak. Bunu Choices ile yapalım kız ve erkek olarak gelsin . Örnek yukarıda(year in school daki gibi)</t>
   </si>
   <si>
-    <t>ad soyad gibi yazılar girilirken ilk harfleri büyük hale getirebiliriz. Kaydetmeden önce</t>
-  </si>
-  <si>
     <t>Cevaplar diye ayrı bir tablo yaratalım. Gerekebilir</t>
   </si>
   <si>
@@ -278,9 +272,6 @@
     <t>sınıf listesi return value de  2021-2022 - 9B gibi yazmalı</t>
   </si>
   <si>
-    <t>öğrenci listesinde öğrenci nosu olacak</t>
-  </si>
-  <si>
     <t>öğrencinin ve kullanıcıların doğum tarihlerini ekleyelim</t>
   </si>
   <si>
@@ -308,21 +299,12 @@
     <t>image resimlerini kaydederken anlamlı olmalı. Ornegin kisinin TC kimlik nosu olabilir</t>
   </si>
   <si>
-    <t>TC alanı cok dar onu genişletmemiz gerekiyor</t>
-  </si>
-  <si>
     <t>Kullanıcılardaki benzer alanlar aynı selikde öğrencide de olacak. Datefield , tc no, telefon vb gibi.</t>
   </si>
   <si>
-    <t>Öğrenci TC alanını Genişlet</t>
-  </si>
-  <si>
     <t>Doğum tarihi datefiled olacak</t>
   </si>
   <si>
-    <t>Ogrenci Ad yok</t>
-  </si>
-  <si>
     <t>Örnek projeler araştırılacak. Tüm iyi yönleri alınacak</t>
   </si>
   <si>
@@ -368,9 +350,6 @@
     <t>Öncelik</t>
   </si>
   <si>
-    <t>DIS verileri dısardan import şeklinde otomatik çekilecek. Bunun için dis verilerin formati öğrenilecek</t>
-  </si>
-  <si>
     <t>Faz 2</t>
   </si>
   <si>
@@ -378,12 +357,6 @@
   </si>
   <si>
     <t>Faz 1</t>
-  </si>
-  <si>
-    <t>Eren</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Yapılmadı</t>
@@ -558,6 +531,18 @@
   </si>
   <si>
     <t>görev tanımı prfil sayfasında otomatik oalrak kayıtlı olan gelmeli</t>
+  </si>
+  <si>
+    <t>Seymen/Ertan</t>
+  </si>
+  <si>
+    <t>DIS verileri dısardan import şeklinde otomatik çekilecek. Bunun için dis verilerin formati öğrenilecek ve sonrasında import edebilmek için bir html safasında o dosya çekilip import işlemi yaptırılacak</t>
+  </si>
+  <si>
+    <t>ad soyad gibi yazılar girilirken ilk harfleri büyük hale getirebiliriz. Kaydetmeden önce sorgulayıp düzeltme yaptırlamım buna clean data diyeceğiz. Djangoda da clean_data var bakmak lazım</t>
+  </si>
+  <si>
+    <t>öğrenci tablosunda  öğrenci nosu olacak</t>
   </si>
 </sst>
 </file>
@@ -737,12 +722,6 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -783,6 +762,12 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -800,92 +785,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1577340</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3017520</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>990245</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Resim 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2186940" y="845820"/>
-          <a:ext cx="1440180" cy="875945"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2231001</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>2083506</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Resim 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="891540" y="4602480"/>
-          <a:ext cx="1949061" cy="1999686"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>55924</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>2457877</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>64301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -895,7 +804,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1116,13 +1025,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tablo1" displayName="Tablo1" ref="A1:F273" totalsRowShown="0">
-  <autoFilter ref="A1:F273"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tablo1" displayName="Tablo1" ref="A1:F270" totalsRowShown="0">
+  <autoFilter ref="A1:F270"/>
+  <sortState ref="A2:F248">
+    <sortCondition ref="F1:F273"/>
+  </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="No"/>
     <tableColumn id="6" name="Konu"/>
-    <tableColumn id="2" name="Yapıalcaklar" dataDxfId="1"/>
-    <tableColumn id="3" name="Öncelik" dataDxfId="0"/>
+    <tableColumn id="2" name="Yapıalcaklar" dataDxfId="6"/>
+    <tableColumn id="3" name="Öncelik" dataDxfId="5"/>
     <tableColumn id="4" name="Kim Yapıyor"/>
     <tableColumn id="5" name="Durumu"/>
   </tableColumns>
@@ -1396,15 +1308,15 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F248"/>
+  <dimension ref="A1:F245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L67" sqref="L67"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.33203125" style="15" customWidth="1"/>
     <col min="4" max="4" width="14.109375" style="15" customWidth="1"/>
@@ -1414,42 +1326,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1458,271 +1355,313 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A66" si="0">A3+1</f>
+        <f>A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>137</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f>A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f>A5+1</f>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>137</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f>A6+1</f>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C7" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>A8+1</f>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" ref="A10:A69" si="0">A9+1</f>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D14" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="204" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>131</v>
-      </c>
       <c r="C17" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E17" t="s">
+        <v>137</v>
       </c>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1731,16 +1670,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E18" t="s">
+        <v>137</v>
       </c>
       <c r="F18" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1749,16 +1691,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E19" t="s">
+        <v>137</v>
       </c>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1767,16 +1712,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E20" t="s">
+        <v>137</v>
       </c>
       <c r="F20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1785,16 +1733,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E21" t="s">
+        <v>137</v>
       </c>
       <c r="F21" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1803,16 +1754,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E22" t="s">
+        <v>137</v>
       </c>
       <c r="F22" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1821,16 +1775,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E23" t="s">
+        <v>137</v>
       </c>
       <c r="F23" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1839,16 +1796,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E24" t="s">
+        <v>137</v>
       </c>
       <c r="F24" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1857,16 +1817,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E25" t="s">
+        <v>137</v>
       </c>
       <c r="F25" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1875,16 +1838,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E26" t="s">
+        <v>137</v>
       </c>
       <c r="F26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1893,16 +1859,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="E27" t="s">
+        <v>137</v>
       </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1911,16 +1880,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>118</v>
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>137</v>
       </c>
       <c r="F28" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1929,1628 +1901,1646 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A33" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" t="s">
+        <v>137</v>
+      </c>
+      <c r="F37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" t="s">
+        <v>137</v>
+      </c>
+      <c r="F38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+      <c r="A39" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="D39" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A40" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B41" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A42" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" t="s">
+        <v>137</v>
+      </c>
+      <c r="F42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A43" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" t="s">
+        <v>137</v>
+      </c>
+      <c r="F43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A44" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D44" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="E44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>139</v>
-      </c>
-      <c r="C36" s="15" t="s">
+      <c r="D45" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" t="s">
+        <v>137</v>
+      </c>
+      <c r="F46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E47" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E48" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" t="s">
+        <v>137</v>
+      </c>
+      <c r="F49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D37" s="15" t="s">
+      <c r="D50" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" t="s">
+        <v>137</v>
+      </c>
+      <c r="F50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="F37" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>139</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F38" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F39" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F41" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="216" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>139</v>
-      </c>
-      <c r="C42" s="15" t="s">
+      <c r="D51" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" t="s">
+        <v>137</v>
+      </c>
+      <c r="F51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C52" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F42" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>139</v>
-      </c>
-      <c r="C43" s="15" t="s">
+      <c r="D52" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" t="s">
+        <v>137</v>
+      </c>
+      <c r="F52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C53" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F43" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>139</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F44" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F45" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F46" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F47" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F48" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F49" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F50" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F53" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F54" t="s">
-        <v>121</v>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F55" t="s">
-        <v>121</v>
+      <c r="A55" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>145</v>
+      <c r="A56" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>56</v>
+      <c r="A57" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>57</v>
+      <c r="A58" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>58</v>
+      <c r="A59" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>59</v>
+      <c r="A60" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>60</v>
+      <c r="A61" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>61</v>
+      <c r="A62" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>62</v>
+      <c r="A63" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <f t="shared" si="0"/>
-        <v>63</v>
+      <c r="A64" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <f t="shared" si="0"/>
-        <v>64</v>
+      <c r="A65" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <f t="shared" si="0"/>
-        <v>65</v>
+      <c r="A66" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <f t="shared" ref="A67:A130" si="1">A66+1</f>
-        <v>66</v>
+      <c r="A67" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <f t="shared" si="1"/>
-        <v>67</v>
+      <c r="A68" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <f t="shared" si="1"/>
-        <v>68</v>
+      <c r="A69" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <f t="shared" si="1"/>
-        <v>69</v>
+      <c r="A70" t="e">
+        <f t="shared" ref="A70:A133" si="1">A69+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <f t="shared" si="1"/>
-        <v>70</v>
+      <c r="A71" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <f t="shared" si="1"/>
-        <v>71</v>
+      <c r="A72" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <f t="shared" si="1"/>
-        <v>72</v>
+      <c r="A73" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <f t="shared" si="1"/>
-        <v>73</v>
+      <c r="A74" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <f t="shared" si="1"/>
-        <v>74</v>
+      <c r="A75" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <f t="shared" si="1"/>
-        <v>75</v>
+      <c r="A76" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <f t="shared" si="1"/>
-        <v>76</v>
+      <c r="A77" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <f t="shared" si="1"/>
-        <v>77</v>
+      <c r="A78" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <f t="shared" si="1"/>
-        <v>78</v>
+      <c r="A79" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <f t="shared" si="1"/>
-        <v>79</v>
+      <c r="A80" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <f t="shared" si="1"/>
-        <v>80</v>
+      <c r="A81" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <f t="shared" si="1"/>
-        <v>81</v>
+      <c r="A82" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <f t="shared" si="1"/>
-        <v>82</v>
+      <c r="A83" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <f t="shared" si="1"/>
-        <v>83</v>
+      <c r="A84" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <f t="shared" si="1"/>
-        <v>84</v>
+      <c r="A85" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <f t="shared" si="1"/>
-        <v>85</v>
+      <c r="A86" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87">
-        <f t="shared" si="1"/>
-        <v>86</v>
+      <c r="A87" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88">
-        <f t="shared" si="1"/>
-        <v>87</v>
+      <c r="A88" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89">
-        <f t="shared" si="1"/>
-        <v>88</v>
+      <c r="A89" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <f t="shared" si="1"/>
-        <v>89</v>
+      <c r="A90" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91">
-        <f t="shared" si="1"/>
-        <v>90</v>
+      <c r="A91" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <f t="shared" si="1"/>
-        <v>91</v>
+      <c r="A92" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <f t="shared" si="1"/>
-        <v>92</v>
+      <c r="A93" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <f t="shared" si="1"/>
-        <v>93</v>
+      <c r="A94" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <f t="shared" si="1"/>
-        <v>94</v>
+      <c r="A95" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <f t="shared" si="1"/>
-        <v>95</v>
+      <c r="A96" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <f t="shared" si="1"/>
-        <v>96</v>
+      <c r="A97" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <f t="shared" si="1"/>
-        <v>97</v>
+      <c r="A98" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <f t="shared" si="1"/>
-        <v>98</v>
+      <c r="A99" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <f t="shared" si="1"/>
-        <v>99</v>
+      <c r="A100" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <f t="shared" si="1"/>
-        <v>100</v>
+      <c r="A101" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <f t="shared" si="1"/>
-        <v>101</v>
+      <c r="A102" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <f t="shared" si="1"/>
-        <v>102</v>
+      <c r="A103" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <f t="shared" si="1"/>
-        <v>103</v>
+      <c r="A104" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <f t="shared" si="1"/>
-        <v>104</v>
+      <c r="A105" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <f t="shared" si="1"/>
-        <v>105</v>
+      <c r="A106" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <f t="shared" si="1"/>
-        <v>106</v>
+      <c r="A107" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <f t="shared" si="1"/>
-        <v>107</v>
+      <c r="A108" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <f t="shared" si="1"/>
-        <v>108</v>
+      <c r="A109" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <f t="shared" si="1"/>
-        <v>109</v>
+      <c r="A110" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111">
-        <f t="shared" si="1"/>
-        <v>110</v>
+      <c r="A111" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112">
-        <f t="shared" si="1"/>
-        <v>111</v>
+      <c r="A112" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113">
-        <f t="shared" si="1"/>
-        <v>112</v>
+      <c r="A113" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114">
-        <f t="shared" si="1"/>
-        <v>113</v>
+      <c r="A114" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115">
-        <f t="shared" si="1"/>
-        <v>114</v>
+      <c r="A115" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116">
-        <f t="shared" si="1"/>
-        <v>115</v>
+      <c r="A116" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <f t="shared" si="1"/>
-        <v>116</v>
+      <c r="A117" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <f t="shared" si="1"/>
-        <v>117</v>
+      <c r="A118" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <f t="shared" si="1"/>
-        <v>118</v>
+      <c r="A119" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <f t="shared" si="1"/>
-        <v>119</v>
+      <c r="A120" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121">
-        <f t="shared" si="1"/>
-        <v>120</v>
+      <c r="A121" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <f t="shared" si="1"/>
-        <v>121</v>
+      <c r="A122" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123">
-        <f t="shared" si="1"/>
-        <v>122</v>
+      <c r="A123" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124">
-        <f t="shared" si="1"/>
-        <v>123</v>
+      <c r="A124" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125">
-        <f t="shared" si="1"/>
-        <v>124</v>
+      <c r="A125" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126">
-        <f t="shared" si="1"/>
-        <v>125</v>
+      <c r="A126" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127">
-        <f t="shared" si="1"/>
-        <v>126</v>
+      <c r="A127" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128">
-        <f t="shared" si="1"/>
-        <v>127</v>
+      <c r="A128" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129">
-        <f t="shared" si="1"/>
-        <v>128</v>
+      <c r="A129" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130">
-        <f t="shared" si="1"/>
-        <v>129</v>
+      <c r="A130" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131">
-        <f t="shared" ref="A131:A194" si="2">A130+1</f>
-        <v>130</v>
+      <c r="A131" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132">
+      <c r="A132" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="e">
+        <f t="shared" ref="A134:A150" si="2">A133+1</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="e">
         <f t="shared" si="2"/>
-        <v>131</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="e">
         <f t="shared" si="2"/>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="e">
         <f t="shared" si="2"/>
-        <v>133</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" t="e">
         <f t="shared" si="2"/>
-        <v>134</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="e">
         <f t="shared" si="2"/>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="e">
         <f t="shared" si="2"/>
-        <v>136</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="e">
         <f t="shared" si="2"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="e">
         <f t="shared" si="2"/>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="e">
         <f t="shared" si="2"/>
-        <v>139</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="e">
         <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="e">
         <f t="shared" si="2"/>
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="e">
         <f t="shared" si="2"/>
-        <v>142</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="e">
         <f t="shared" si="2"/>
-        <v>143</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="e">
         <f t="shared" si="2"/>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="e">
         <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="e">
         <f t="shared" si="2"/>
-        <v>146</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148">
-        <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149">
-        <f t="shared" si="2"/>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150">
-        <f t="shared" si="2"/>
-        <v>149</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151">
-        <f t="shared" si="2"/>
-        <v>150</v>
+      <c r="A151" t="e">
+        <f>A150+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152">
-        <f t="shared" si="2"/>
-        <v>151</v>
+      <c r="A152" t="e">
+        <f>A151+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153">
-        <f t="shared" si="2"/>
-        <v>152</v>
+      <c r="A153" t="e">
+        <f>A152+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154">
-        <f t="shared" si="2"/>
-        <v>153</v>
+      <c r="A154" t="e">
+        <f>A153+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155">
-        <f t="shared" si="2"/>
-        <v>154</v>
+      <c r="A155" t="e">
+        <f>A154+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156">
-        <f t="shared" si="2"/>
-        <v>155</v>
+      <c r="A156" t="e">
+        <f>A155+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157">
-        <f t="shared" si="2"/>
-        <v>156</v>
+      <c r="A157" t="e">
+        <f>A156+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158">
-        <f t="shared" si="2"/>
-        <v>157</v>
+      <c r="A158" t="e">
+        <f>A157+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159">
-        <f t="shared" si="2"/>
-        <v>158</v>
+      <c r="A159" t="e">
+        <f>A158+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160">
-        <f t="shared" si="2"/>
-        <v>159</v>
+      <c r="A160" t="e">
+        <f>A159+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161">
-        <f t="shared" si="2"/>
-        <v>160</v>
+      <c r="A161" t="e">
+        <f>A160+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162">
-        <f t="shared" si="2"/>
-        <v>161</v>
+      <c r="A162" t="e">
+        <f>A161+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163">
-        <f t="shared" si="2"/>
-        <v>162</v>
+      <c r="A163" t="e">
+        <f>A162+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164">
-        <f t="shared" si="2"/>
-        <v>163</v>
+      <c r="A164" t="e">
+        <f>A163+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165">
-        <f t="shared" si="2"/>
-        <v>164</v>
+      <c r="A165" t="e">
+        <f>A164+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166">
-        <f t="shared" si="2"/>
-        <v>165</v>
+      <c r="A166" t="e">
+        <f>A165+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167">
-        <f t="shared" si="2"/>
-        <v>166</v>
+      <c r="A167" t="e">
+        <f>A166+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168">
-        <f t="shared" si="2"/>
-        <v>167</v>
+      <c r="A168" t="e">
+        <f>A167+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169">
-        <f t="shared" si="2"/>
-        <v>168</v>
+      <c r="A169" t="e">
+        <f>A168+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170">
-        <f t="shared" si="2"/>
-        <v>169</v>
+      <c r="A170" t="e">
+        <f>A169+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171">
-        <f t="shared" si="2"/>
-        <v>170</v>
+      <c r="A171" t="e">
+        <f>A170+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172">
-        <f t="shared" si="2"/>
-        <v>171</v>
+      <c r="A172" t="e">
+        <f>A171+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173">
-        <f t="shared" si="2"/>
-        <v>172</v>
+      <c r="A173" t="e">
+        <f>A172+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A174">
-        <f t="shared" si="2"/>
-        <v>173</v>
+      <c r="A174" t="e">
+        <f>A173+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A175">
-        <f t="shared" si="2"/>
-        <v>174</v>
+      <c r="A175" t="e">
+        <f>A174+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A176">
-        <f t="shared" si="2"/>
-        <v>175</v>
+      <c r="A176" t="e">
+        <f>A175+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177">
-        <f t="shared" si="2"/>
-        <v>176</v>
+      <c r="A177" t="e">
+        <f>A176+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178">
-        <f t="shared" si="2"/>
-        <v>177</v>
+      <c r="A178" t="e">
+        <f>A177+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A179">
-        <f t="shared" si="2"/>
-        <v>178</v>
+      <c r="A179" t="e">
+        <f>A178+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180">
-        <f t="shared" si="2"/>
-        <v>179</v>
+      <c r="A180" t="e">
+        <f>A179+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A181">
-        <f t="shared" si="2"/>
-        <v>180</v>
+      <c r="A181" t="e">
+        <f>A180+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A182">
-        <f t="shared" si="2"/>
-        <v>181</v>
+      <c r="A182" t="e">
+        <f>A181+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A183">
-        <f t="shared" si="2"/>
-        <v>182</v>
+      <c r="A183" t="e">
+        <f>A182+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A184">
-        <f t="shared" si="2"/>
-        <v>183</v>
+      <c r="A184" t="e">
+        <f>A183+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A185">
-        <f t="shared" si="2"/>
-        <v>184</v>
+      <c r="A185" t="e">
+        <f>A184+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A186">
-        <f t="shared" si="2"/>
-        <v>185</v>
+      <c r="A186" t="e">
+        <f>A185+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A187">
-        <f t="shared" si="2"/>
-        <v>186</v>
+      <c r="A187" t="e">
+        <f>A186+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A188">
-        <f t="shared" si="2"/>
-        <v>187</v>
+      <c r="A188" t="e">
+        <f>A187+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A189">
-        <f t="shared" si="2"/>
-        <v>188</v>
+      <c r="A189" t="e">
+        <f>A188+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A190">
-        <f t="shared" si="2"/>
-        <v>189</v>
+      <c r="A190" t="e">
+        <f>A189+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A191">
-        <f t="shared" si="2"/>
-        <v>190</v>
+      <c r="A191" t="e">
+        <f>A190+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A192">
-        <f t="shared" si="2"/>
-        <v>191</v>
+      <c r="A192" t="e">
+        <f>A191+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A193">
-        <f t="shared" si="2"/>
-        <v>192</v>
+      <c r="A193" t="e">
+        <f>A192+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A194">
-        <f t="shared" si="2"/>
-        <v>193</v>
+      <c r="A194" t="e">
+        <f>A193+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A195">
-        <f t="shared" ref="A195:A248" si="3">A194+1</f>
-        <v>194</v>
+      <c r="A195" t="e">
+        <f>A194+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196">
-        <f t="shared" si="3"/>
-        <v>195</v>
+      <c r="A196" t="e">
+        <f>A195+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A197">
-        <f t="shared" si="3"/>
-        <v>196</v>
+      <c r="A197" t="e">
+        <f>A196+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A198">
-        <f t="shared" si="3"/>
-        <v>197</v>
+      <c r="A198" t="e">
+        <f>A197+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A199">
-        <f t="shared" si="3"/>
-        <v>198</v>
+      <c r="A199" t="e">
+        <f>A198+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A200">
-        <f t="shared" si="3"/>
-        <v>199</v>
+      <c r="A200" t="e">
+        <f>A199+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A201">
-        <f t="shared" si="3"/>
-        <v>200</v>
+      <c r="A201" t="e">
+        <f>A200+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A202">
-        <f t="shared" si="3"/>
-        <v>201</v>
+      <c r="A202" t="e">
+        <f>A201+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A203">
-        <f t="shared" si="3"/>
-        <v>202</v>
+      <c r="A203" t="e">
+        <f>A202+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A204">
-        <f t="shared" si="3"/>
-        <v>203</v>
+      <c r="A204" t="e">
+        <f>A203+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A205">
-        <f t="shared" si="3"/>
-        <v>204</v>
+      <c r="A205" t="e">
+        <f>A204+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A206">
-        <f t="shared" si="3"/>
-        <v>205</v>
+      <c r="A206" t="e">
+        <f>A205+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A207">
-        <f t="shared" si="3"/>
-        <v>206</v>
+      <c r="A207" t="e">
+        <f>A206+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A208">
-        <f t="shared" si="3"/>
-        <v>207</v>
+      <c r="A208" t="e">
+        <f>A207+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A209">
-        <f t="shared" si="3"/>
-        <v>208</v>
+      <c r="A209" t="e">
+        <f>A208+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A210">
-        <f t="shared" si="3"/>
-        <v>209</v>
+      <c r="A210" t="e">
+        <f>A209+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A211">
-        <f t="shared" si="3"/>
-        <v>210</v>
+      <c r="A211" t="e">
+        <f>A210+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A212">
-        <f t="shared" si="3"/>
-        <v>211</v>
+      <c r="A212" t="e">
+        <f>A211+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A213">
-        <f t="shared" si="3"/>
-        <v>212</v>
+      <c r="A213" t="e">
+        <f>A212+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A214">
-        <f t="shared" si="3"/>
-        <v>213</v>
+      <c r="A214" t="e">
+        <f>A213+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A215">
-        <f t="shared" si="3"/>
-        <v>214</v>
+      <c r="A215" t="e">
+        <f>A214+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A216">
-        <f t="shared" si="3"/>
-        <v>215</v>
+      <c r="A216" t="e">
+        <f>A215+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A217">
-        <f t="shared" si="3"/>
-        <v>216</v>
+      <c r="A217" t="e">
+        <f>A216+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A218">
-        <f t="shared" si="3"/>
-        <v>217</v>
+      <c r="A218" t="e">
+        <f>A217+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A219">
-        <f t="shared" si="3"/>
-        <v>218</v>
+      <c r="A219" t="e">
+        <f>A218+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A220">
-        <f t="shared" si="3"/>
-        <v>219</v>
+      <c r="A220" t="e">
+        <f>A219+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A221">
-        <f t="shared" si="3"/>
-        <v>220</v>
+      <c r="A221" t="e">
+        <f>A220+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A222">
-        <f t="shared" si="3"/>
-        <v>221</v>
+      <c r="A222" t="e">
+        <f>A221+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A223">
-        <f t="shared" si="3"/>
-        <v>222</v>
+      <c r="A223" t="e">
+        <f>A222+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A224">
-        <f t="shared" si="3"/>
-        <v>223</v>
+      <c r="A224" t="e">
+        <f>A223+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A225">
-        <f t="shared" si="3"/>
-        <v>224</v>
+      <c r="A225" t="e">
+        <f>A224+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A226">
-        <f t="shared" si="3"/>
-        <v>225</v>
+      <c r="A226" t="e">
+        <f>A225+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A227">
-        <f t="shared" si="3"/>
-        <v>226</v>
+      <c r="A227" t="e">
+        <f>A226+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A228">
-        <f t="shared" si="3"/>
-        <v>227</v>
+      <c r="A228" t="e">
+        <f>A227+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A229">
-        <f t="shared" si="3"/>
-        <v>228</v>
+      <c r="A229" t="e">
+        <f>A228+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A230">
-        <f t="shared" si="3"/>
-        <v>229</v>
+      <c r="A230" t="e">
+        <f>A229+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A231">
-        <f t="shared" si="3"/>
-        <v>230</v>
+      <c r="A231" t="e">
+        <f>A230+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A232">
-        <f t="shared" si="3"/>
-        <v>231</v>
+      <c r="A232" t="e">
+        <f>A231+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A233">
-        <f t="shared" si="3"/>
-        <v>232</v>
+      <c r="A233" t="e">
+        <f>A232+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A234">
-        <f t="shared" si="3"/>
-        <v>233</v>
+      <c r="A234" t="e">
+        <f>A233+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A235">
-        <f t="shared" si="3"/>
-        <v>234</v>
+      <c r="A235" t="e">
+        <f>A234+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A236">
-        <f t="shared" si="3"/>
-        <v>235</v>
+      <c r="A236" t="e">
+        <f>A235+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A237">
-        <f t="shared" si="3"/>
-        <v>236</v>
+      <c r="A237" t="e">
+        <f>A236+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A238">
-        <f t="shared" si="3"/>
-        <v>237</v>
+      <c r="A238" t="e">
+        <f>A237+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A239">
-        <f t="shared" si="3"/>
-        <v>238</v>
+      <c r="A239" t="e">
+        <f>A238+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A240">
-        <f t="shared" si="3"/>
-        <v>239</v>
+      <c r="A240" t="e">
+        <f>A239+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A241">
-        <f t="shared" si="3"/>
-        <v>240</v>
+      <c r="A241" t="e">
+        <f>A240+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A242">
-        <f t="shared" si="3"/>
-        <v>241</v>
+      <c r="A242" t="e">
+        <f>A241+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A243">
-        <f t="shared" si="3"/>
-        <v>242</v>
+      <c r="A243" t="e">
+        <f>A242+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A244">
-        <f t="shared" si="3"/>
-        <v>243</v>
+      <c r="A244" t="e">
+        <f>A243+1</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A245">
-        <f t="shared" si="3"/>
-        <v>244</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A246">
-        <f t="shared" si="3"/>
-        <v>245</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A247">
-        <f t="shared" si="3"/>
-        <v>246</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A248">
-        <f t="shared" si="3"/>
-        <v>247</v>
+      <c r="A245" t="e">
+        <f>A244+1</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Yapıldı"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"Yapılmadı"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Faz 3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"Faz 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"Faz 1"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4222,7 +4212,7 @@
     <row r="87" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="4"/>
@@ -4230,10 +4220,10 @@
     <row r="89" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B89" s="9"/>
       <c r="C89" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade navbar perod and session
</commit_message>
<xml_diff>
--- a/Yapılacaklar.xlsx
+++ b/Yapılacaklar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="8664" windowWidth="22260" windowHeight="12648" tabRatio="555"/>
+    <workbookView xWindow="0" yWindow="9120" windowWidth="22260" windowHeight="12648" tabRatio="555" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Yapilacaklar" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="129">
   <si>
     <t>Kullanıcılar</t>
   </si>
@@ -227,30 +227,9 @@
     <t>geç geldi/gelmedi/izinli/raporlu/raporsuz</t>
   </si>
   <si>
-    <t>dönem yillar texfield charfield olacak ve limitlenecek burada  default olarak o yılın donemi gelebilir 2021-2022 gibi</t>
-  </si>
-  <si>
-    <t>kullanıcılarda ilişki düzelecek birden falza kişi aynı bransı secebilecek</t>
-  </si>
-  <si>
-    <t>telefonda limit olacak ve validasyon yapacağız</t>
-  </si>
-  <si>
     <t>tüm modellerin (tabloların ) return valueları düzenlenecek. Mantıklı hale getirilecek. Örneğin öğrenci listesinde ad ve soyad görünebilinir.</t>
   </si>
   <si>
-    <t>kullanıcılar(admin) de email var ilişkilendirilince zaten bağlanmış olacak ancak öğrenciler içinde email koyalım</t>
-  </si>
-  <si>
-    <t>emailler emailFİeld olacak</t>
-  </si>
-  <si>
-    <t>öğrencilerde ve kullanıcılarda cinsiyet olacak. Bunu Choices ile yapalım kız ve erkek olarak gelsin . Örnek yukarıda(year in school daki gibi)</t>
-  </si>
-  <si>
-    <t>Cevaplar diye ayrı bir tablo yaratalım. Gerekebilir</t>
-  </si>
-  <si>
     <t>Cevaplar</t>
   </si>
   <si>
@@ -260,15 +239,6 @@
     <t>charfield limitli</t>
   </si>
   <si>
-    <t>rapor ogrenciyi yanlıs anlamıssın. Burada rapor türü olarak DIS, Anket veya not raporu istenebilir. Öğrenci secilecek. Burayı henüz kafamda netleştiremedim buna bakarız ama komple değişecek</t>
-  </si>
-  <si>
-    <t>rapor sınıfta aynı sekilde</t>
-  </si>
-  <si>
-    <t>sınıf listesinde sınıf no min 9 maksimum 12 olacak bunu da choices ile yapabiliriz</t>
-  </si>
-  <si>
     <t>sınıf listesi return value de  2021-2022 - 9B gibi yazmalı</t>
   </si>
   <si>
@@ -293,12 +263,6 @@
     <t>hes kodunun bir formatı var ona uygun olmalı. Bunu da form sayfasında Txxx-xxx-x gibi formatta göstereceğiz</t>
   </si>
   <si>
-    <t>resimler images altına atılıyor. Ole değilde resmi veri tabanına kodlayarak gömelim. Binarry kodla kaydeidlecek. Bu arastırılacak</t>
-  </si>
-  <si>
-    <t>image resimlerini kaydederken anlamlı olmalı. Ornegin kisinin TC kimlik nosu olabilir</t>
-  </si>
-  <si>
     <t>Kullanıcılardaki benzer alanlar aynı selikde öğrencide de olacak. Datefield , tc no, telefon vb gibi.</t>
   </si>
   <si>
@@ -308,9 +272,6 @@
     <t>Örnek projeler araştırılacak. Tüm iyi yönleri alınacak</t>
   </si>
   <si>
-    <t>Veli görüşmesi için randevu sistemi</t>
-  </si>
-  <si>
     <t>Öğrenci servisi atama sayfası</t>
   </si>
   <si>
@@ -350,9 +311,6 @@
     <t>Faz 2</t>
   </si>
   <si>
-    <t>Anket listesi yapılacak anket araştırmalrına göre güncellenecek</t>
-  </si>
-  <si>
     <t>Faz 1</t>
   </si>
   <si>
@@ -390,9 +348,6 @@
   </si>
   <si>
     <t>views</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yoklama sayfası eklenecek. Önce içeriği tasarlanacak ve HTML sayfası oluşturulacak. Daha sonra arka plan kodlamasına geçilecek. Örnek olarak yoklama sayfasına tıkladığında popup veya gelen sayfada en üstte sınıfı seçsin hemen altında da ders saatini seçsin . Hemen altta bir tablo olsun ve bu tabloda seçtiği sınıfın öğrencileri listelensin. tablonun en sağında ise Var ve yok (veya tick) butonları olsun. en altta da kaydet olsun. Bunun için yoklama listesi diye bir veritabanı modeli yaratacağız. içersinde öğrenci , dönem,ders saati sınıf,durum bilgisi olacak. Ders saatleri için yine bir veri tabanı modeli oluşturacağız. 1.Ders - 9.30 - 10:10 gibi. </t>
   </si>
   <si>
     <t>Faz 3</t>
@@ -533,9 +488,6 @@
     <t>DIS verileri dısardan import şeklinde otomatik çekilecek. Bunun için dis verilerin formati öğrenilecek ve sonrasında import edebilmek için bir html safasında o dosya çekilip import işlemi yaptırılacak</t>
   </si>
   <si>
-    <t>ad soyad gibi yazılar girilirken ilk harfleri büyük hale getirebiliriz. Kaydetmeden önce sorgulayıp düzeltme yaptırlamım buna clean data diyeceğiz. Djangoda da clean_data var bakmak lazım</t>
-  </si>
-  <si>
     <t>öğrenci tablosunda  öğrenci nosu olacak</t>
   </si>
   <si>
@@ -552,6 +504,9 @@
   </si>
   <si>
     <t>cinsiyet seçimi bu şekilde olabiliir ve tarih seçimide datepciker şeklinde acılan pencereden yapılacak. https://django-datta-able-pro.appseed-srv1.com/auth-personal-information.html</t>
+  </si>
+  <si>
+    <t>w37</t>
   </si>
 </sst>
 </file>
@@ -802,8 +757,8 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>55924</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>64301</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>73266</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1471,8 +1426,8 @@
   </sheetPr>
   <dimension ref="A1:F245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1487,22 +1442,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1510,2188 +1465,2138 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <f t="shared" ref="A3:A9" si="0">A2+1</f>
-        <v>2</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="e">
+        <f t="shared" ref="A3:A9" si="0">A3+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="e">
+        <f t="shared" ref="A10:A73" si="1">A9+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="D14" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="15" t="s">
+      <c r="D19" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="15" t="s">
+      <c r="D21" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E9" t="s">
-        <v>135</v>
-      </c>
-      <c r="F9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" ref="A10:A73" si="1">A9+1</f>
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="15" t="s">
+      <c r="D22" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B24" t="s">
         <v>108</v>
       </c>
-      <c r="E10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="C24" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B25" t="s">
         <v>108</v>
       </c>
-      <c r="E11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" t="s">
-        <v>135</v>
-      </c>
-      <c r="F15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="15" t="s">
+      <c r="C25" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E17" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" t="s">
-        <v>135</v>
-      </c>
-      <c r="F20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" t="s">
-        <v>135</v>
-      </c>
-      <c r="F21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F24" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="D25" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F25" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <f t="shared" si="1"/>
-        <v>25</v>
+      <c r="A26" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F28" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E29" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F29" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F30" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F31" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F32" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F33" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E34" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F34" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E35" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F35" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C36" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" t="s">
         <v>97</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E36" t="s">
-        <v>135</v>
-      </c>
-      <c r="F36" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F37" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E38" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F38" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E39" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F39" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F40" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E41" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F41" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F42" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E43" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F43" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E44" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F44" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F45" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E46" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F46" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E47" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F47" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E48" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F48" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F49" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E50" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F50" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E51" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F51" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E52" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F52" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="223.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="222.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" ref="A74:A121" si="2">A73+1</f>
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="2"/>
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="2"/>
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="2"/>
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="2"/>
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="2"/>
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="2"/>
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="2"/>
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="2"/>
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="2"/>
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="2"/>
-        <v>91</v>
+        <v>72</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="2"/>
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="2"/>
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="2"/>
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="2"/>
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="2"/>
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
         <f t="shared" si="2"/>
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
         <f t="shared" si="2"/>
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
         <f t="shared" si="2"/>
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
         <f t="shared" si="2"/>
-        <v>105</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
         <f t="shared" si="2"/>
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
         <f t="shared" si="2"/>
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
         <f t="shared" si="2"/>
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
         <f t="shared" si="2"/>
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
         <f t="shared" si="2"/>
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
         <f t="shared" si="2"/>
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
         <f t="shared" si="2"/>
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
         <f t="shared" si="2"/>
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
         <f t="shared" si="2"/>
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
         <f t="shared" si="2"/>
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
         <f t="shared" si="2"/>
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
         <f t="shared" si="2"/>
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
         <f t="shared" si="2"/>
-        <v>118</v>
+        <v>99</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
         <f t="shared" si="2"/>
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121">
         <f t="shared" si="2"/>
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
         <f t="shared" ref="A122:A133" si="3">A121+1</f>
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>103</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
         <f t="shared" si="3"/>
-        <v>123</v>
+        <v>104</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
         <f t="shared" si="3"/>
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
         <f t="shared" si="3"/>
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
         <f t="shared" si="3"/>
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
         <f t="shared" si="3"/>
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
         <f t="shared" ref="A134:A150" si="4">A133+1</f>
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
         <f t="shared" si="4"/>
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
         <f t="shared" si="4"/>
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
         <f t="shared" si="4"/>
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
         <f t="shared" si="4"/>
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
         <f t="shared" si="4"/>
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
         <f t="shared" si="4"/>
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141">
         <f t="shared" si="4"/>
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
         <f t="shared" si="4"/>
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143">
         <f t="shared" si="4"/>
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144">
         <f t="shared" si="4"/>
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145">
         <f t="shared" si="4"/>
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
         <f t="shared" si="4"/>
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
         <f t="shared" si="4"/>
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
         <f t="shared" si="4"/>
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
         <f t="shared" si="4"/>
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
         <f t="shared" si="4"/>
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151">
         <f t="shared" ref="A151:A182" si="5">A150+1</f>
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
         <f t="shared" si="5"/>
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153">
         <f t="shared" si="5"/>
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
         <f t="shared" si="5"/>
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
         <f t="shared" si="5"/>
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
         <f t="shared" si="5"/>
-        <v>156</v>
+        <v>137</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
         <f t="shared" si="5"/>
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
         <f t="shared" si="5"/>
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
         <f t="shared" si="5"/>
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
         <f t="shared" si="5"/>
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
         <f t="shared" si="5"/>
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163">
         <f t="shared" si="5"/>
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
         <f t="shared" si="5"/>
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
         <f t="shared" si="5"/>
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
         <f t="shared" si="5"/>
-        <v>165</v>
+        <v>146</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
         <f t="shared" si="5"/>
-        <v>166</v>
+        <v>147</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
         <f t="shared" si="5"/>
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
         <f t="shared" si="5"/>
-        <v>168</v>
+        <v>149</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
         <f t="shared" si="5"/>
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
         <f t="shared" si="5"/>
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
         <f t="shared" si="5"/>
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173">
         <f t="shared" si="5"/>
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
         <f t="shared" si="5"/>
-        <v>173</v>
+        <v>154</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
         <f t="shared" si="5"/>
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
         <f t="shared" si="5"/>
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
         <f t="shared" si="5"/>
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
         <f t="shared" si="5"/>
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
         <f t="shared" si="5"/>
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
         <f t="shared" si="5"/>
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
         <f t="shared" si="5"/>
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
         <f t="shared" ref="A183:A214" si="6">A182+1</f>
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
         <f t="shared" si="6"/>
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
         <f t="shared" si="6"/>
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
         <f t="shared" si="6"/>
-        <v>185</v>
+        <v>166</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
         <f t="shared" si="6"/>
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
         <f t="shared" si="6"/>
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
         <f t="shared" si="6"/>
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
         <f t="shared" si="6"/>
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
         <f t="shared" si="6"/>
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
         <f t="shared" si="6"/>
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
         <f t="shared" si="6"/>
-        <v>192</v>
+        <v>173</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
         <f t="shared" si="6"/>
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
         <f t="shared" si="6"/>
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
         <f t="shared" si="6"/>
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
         <f t="shared" si="6"/>
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
         <f t="shared" si="6"/>
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
         <f t="shared" si="6"/>
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
         <f t="shared" si="6"/>
-        <v>199</v>
+        <v>180</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
         <f t="shared" si="6"/>
-        <v>200</v>
+        <v>181</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
         <f t="shared" si="6"/>
-        <v>201</v>
+        <v>182</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
         <f t="shared" si="6"/>
-        <v>202</v>
+        <v>183</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
         <f t="shared" si="6"/>
-        <v>203</v>
+        <v>184</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
         <f t="shared" si="6"/>
-        <v>204</v>
+        <v>185</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
         <f t="shared" si="6"/>
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
         <f t="shared" si="6"/>
-        <v>206</v>
+        <v>187</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
         <f t="shared" si="6"/>
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
         <f t="shared" si="6"/>
-        <v>208</v>
+        <v>189</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
         <f t="shared" si="6"/>
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211">
         <f t="shared" si="6"/>
-        <v>210</v>
+        <v>191</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212">
         <f t="shared" si="6"/>
-        <v>211</v>
+        <v>192</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213">
         <f t="shared" si="6"/>
-        <v>212</v>
+        <v>193</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
         <f t="shared" si="6"/>
-        <v>213</v>
+        <v>194</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
         <f t="shared" ref="A215:A245" si="7">A214+1</f>
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
         <f t="shared" si="7"/>
-        <v>215</v>
+        <v>196</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
         <f t="shared" si="7"/>
-        <v>216</v>
+        <v>197</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
         <f t="shared" si="7"/>
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
         <f t="shared" si="7"/>
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
         <f t="shared" si="7"/>
-        <v>219</v>
+        <v>200</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221">
         <f t="shared" si="7"/>
-        <v>220</v>
+        <v>201</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222">
         <f t="shared" si="7"/>
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223">
         <f t="shared" si="7"/>
-        <v>222</v>
+        <v>203</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
         <f t="shared" si="7"/>
-        <v>223</v>
+        <v>204</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
         <f t="shared" si="7"/>
-        <v>224</v>
+        <v>205</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
         <f t="shared" si="7"/>
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227">
         <f t="shared" si="7"/>
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
         <f t="shared" si="7"/>
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
         <f t="shared" si="7"/>
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
         <f t="shared" si="7"/>
-        <v>229</v>
+        <v>210</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231">
         <f t="shared" si="7"/>
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
         <f t="shared" si="7"/>
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233">
         <f t="shared" si="7"/>
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
         <f t="shared" si="7"/>
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
         <f t="shared" si="7"/>
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
         <f t="shared" si="7"/>
-        <v>235</v>
+        <v>216</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237">
         <f t="shared" si="7"/>
-        <v>236</v>
+        <v>217</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
         <f t="shared" si="7"/>
-        <v>237</v>
+        <v>218</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
         <f t="shared" si="7"/>
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
         <f t="shared" si="7"/>
-        <v>239</v>
+        <v>220</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241">
         <f t="shared" si="7"/>
-        <v>240</v>
+        <v>221</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242">
         <f t="shared" si="7"/>
-        <v>241</v>
+        <v>222</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243">
         <f t="shared" si="7"/>
-        <v>242</v>
+        <v>223</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244">
         <f t="shared" si="7"/>
-        <v>243</v>
+        <v>224</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
         <f t="shared" si="7"/>
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -4382,7 +4287,7 @@
     <row r="87" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="4"/>
@@ -4390,10 +4295,10 @@
     <row r="89" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B89" s="9"/>
       <c r="C89" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4406,7 +4311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>

</xml_diff>